<commit_message>
Preparation for new Antera results
</commit_message>
<xml_diff>
--- a/Data/Antera_inputs_v3.xlsx
+++ b/Data/Antera_inputs_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giparoli\Documents\Projetos\AEco\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AF4E40-AA7A-4F8E-9855-863EF50360DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62987586-3443-454D-A148-1BFAD72C1CDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Antera_spray_etanol" sheetId="11" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Antera_imaging" sheetId="10" r:id="rId3"/>
     <sheet name="Antera_corrective" sheetId="15" r:id="rId4"/>
     <sheet name="Antera_updated" sheetId="16" r:id="rId5"/>
+    <sheet name="Antera_og" sheetId="17" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -637,8 +638,125 @@
 </comments>
 </file>
 
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={8DB2EE64-C56A-4F7C-B3CF-F9588BD29FA5}</author>
+    <author>tc={551FC638-FC81-4F95-A386-B97501001BAA}</author>
+    <author>tc={32C2A301-87BB-480A-AA49-BD24D17B3EF0}</author>
+    <author>tc={547CD471-57E3-4500-8678-BF9B3BDBB476}</author>
+    <author>tc={781393D1-5860-477A-8AB5-081E1AFAA9E3}</author>
+    <author>tc={888B73DA-A041-44A1-817D-B5722BF7FA4B}</author>
+    <author>tc={5C5471B3-12B3-4EE1-B2FC-BBF066D94B0F}</author>
+    <author>tc={313D5D05-2245-4384-A9AE-9D1708216242}</author>
+    <author>tc={CF2FFC56-7757-4FA6-8C60-54BC447E57A2}</author>
+    <author>tc={B8CC286B-13CA-4D0B-B2A5-F5D7AB75B692}</author>
+    <author>tc={59E1C637-75D9-4BEF-B064-CCBC5B61BEFB}</author>
+    <author>tc={6E62DECF-2988-4A4A-9803-744B9D3906AC}</author>
+  </authors>
+  <commentList>
+    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{8DB2EE64-C56A-4F7C-B3CF-F9588BD29FA5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    107087 kWh/month @ G1170. Considering 500 workers in the building, the average per worker is 214.17.</t>
+      </text>
+    </comment>
+    <comment ref="C23" authorId="1" shapeId="0" xr:uid="{551FC638-FC81-4F95-A386-B97501001BAA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    190 m³/month @ G1170. Considering 500 workers in the building, the average per worker is 0.38</t>
+      </text>
+    </comment>
+    <comment ref="C24" authorId="2" shapeId="0" xr:uid="{32C2A301-87BB-480A-AA49-BD24D17B3EF0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    750 m³/month @ G1170. Considering 500 workers in the building, the average per worker is 1.5</t>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="3" shapeId="0" xr:uid="{547CD471-57E3-4500-8678-BF9B3BDBB476}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Rebitadeira automática</t>
+      </text>
+    </comment>
+    <comment ref="C30" authorId="4" shapeId="0" xr:uid="{781393D1-5860-477A-8AB5-081E1AFAA9E3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Considerando 3 estufas (composto), 1 rebitadeiras automáticas, 1 robô pintura, 2 CNC (portas e furos), 1 robô pick and place (composto)</t>
+      </text>
+    </comment>
+    <comment ref="C49" authorId="5" shapeId="0" xr:uid="{888B73DA-A041-44A1-817D-B5722BF7FA4B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    80000 kWh/month @ G1360. Considering 18000 m², the average per m² is 4.44</t>
+      </text>
+    </comment>
+    <comment ref="C50" authorId="6" shapeId="0" xr:uid="{5C5471B3-12B3-4EE1-B2FC-BBF066D94B0F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    80 m³/month @ G1360. Considering 18000 m², the average per m² is 0.00444</t>
+      </text>
+    </comment>
+    <comment ref="C51" authorId="7" shapeId="0" xr:uid="{313D5D05-2245-4384-A9AE-9D1708216242}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    64 m³/month @ G1360. Considering 18000 m², the average per m² is 0.00356</t>
+      </text>
+    </comment>
+    <comment ref="C52" authorId="8" shapeId="0" xr:uid="{CF2FFC56-7757-4FA6-8C60-54BC447E57A2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    0.27 m³/month @ G1360. Considering 18000 m², the average per m² is 0.000015</t>
+      </text>
+    </comment>
+    <comment ref="C54" authorId="9" shapeId="0" xr:uid="{B8CC286B-13CA-4D0B-B2A5-F5D7AB75B692}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Considerando que a distância média de entrega no BR é 800km, extrapolando esse valor para os outros destinos também (considerando que além do transporte marítmo, será enviado via terra até o cliente final)</t>
+      </text>
+    </comment>
+    <comment ref="C57" authorId="10" shapeId="0" xr:uid="{59E1C637-75D9-4BEF-B064-CCBC5B61BEFB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    MTOW em t</t>
+      </text>
+    </comment>
+    <comment ref="C59" authorId="11" shapeId="0" xr:uid="{6E62DECF-2988-4A4A-9803-744B9D3906AC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Em cada container cabem 4 aviões, porém vários componentes serão integrados nos EUA, portanto considerei 70% do MTOW</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="243">
   <si>
     <t>nominal</t>
   </si>
@@ -1401,7 +1519,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1455,6 +1573,12 @@
       <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="12">
@@ -2348,6 +2472,47 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment6.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C22" dT="2019-12-31T13:50:55.89" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{8DB2EE64-C56A-4F7C-B3CF-F9588BD29FA5}">
+    <text>107087 kWh/month @ G1170. Considering 500 workers in the building, the average per worker is 214.17.</text>
+  </threadedComment>
+  <threadedComment ref="C23" dT="2019-12-31T14:01:21.91" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{551FC638-FC81-4F95-A386-B97501001BAA}">
+    <text>190 m³/month @ G1170. Considering 500 workers in the building, the average per worker is 0.38</text>
+  </threadedComment>
+  <threadedComment ref="C24" dT="2019-12-31T14:02:51.19" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{32C2A301-87BB-480A-AA49-BD24D17B3EF0}">
+    <text>750 m³/month @ G1170. Considering 500 workers in the building, the average per worker is 1.5</text>
+  </threadedComment>
+  <threadedComment ref="C29" dT="2021-06-08T03:06:52.41" personId="{172B4ACD-BB32-3A40-A6EE-78502C39DADA}" id="{547CD471-57E3-4500-8678-BF9B3BDBB476}">
+    <text>Rebitadeira automática</text>
+  </threadedComment>
+  <threadedComment ref="C30" dT="2021-06-07T19:51:07.06" personId="{172B4ACD-BB32-3A40-A6EE-78502C39DADA}" id="{781393D1-5860-477A-8AB5-081E1AFAA9E3}">
+    <text>Considerando 3 estufas (composto), 1 rebitadeiras automáticas, 1 robô pintura, 2 CNC (portas e furos), 1 robô pick and place (composto)</text>
+  </threadedComment>
+  <threadedComment ref="C49" dT="2019-12-31T14:53:25.54" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{888B73DA-A041-44A1-817D-B5722BF7FA4B}">
+    <text>80000 kWh/month @ G1360. Considering 18000 m², the average per m² is 4.44</text>
+  </threadedComment>
+  <threadedComment ref="C50" dT="2019-12-31T14:55:29.34" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{5C5471B3-12B3-4EE1-B2FC-BBF066D94B0F}">
+    <text>80 m³/month @ G1360. Considering 18000 m², the average per m² is 0.00444</text>
+  </threadedComment>
+  <threadedComment ref="C51" dT="2019-12-31T16:34:31.50" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{313D5D05-2245-4384-A9AE-9D1708216242}">
+    <text>64 m³/month @ G1360. Considering 18000 m², the average per m² is 0.00356</text>
+  </threadedComment>
+  <threadedComment ref="C52" dT="2019-12-31T16:35:39.91" personId="{6499F404-6823-40DC-996D-949B978ABBF0}" id="{CF2FFC56-7757-4FA6-8C60-54BC447E57A2}">
+    <text>0.27 m³/month @ G1360. Considering 18000 m², the average per m² is 0.000015</text>
+  </threadedComment>
+  <threadedComment ref="C54" dT="2021-06-07T18:01:09.55" personId="{172B4ACD-BB32-3A40-A6EE-78502C39DADA}" id="{B8CC286B-13CA-4D0B-B2A5-F5D7AB75B692}">
+    <text>Considerando que a distância média de entrega no BR é 800km, extrapolando esse valor para os outros destinos também (considerando que além do transporte marítmo, será enviado via terra até o cliente final)</text>
+  </threadedComment>
+  <threadedComment ref="C57" dT="2021-06-07T18:31:21.06" personId="{172B4ACD-BB32-3A40-A6EE-78502C39DADA}" id="{59E1C637-75D9-4BEF-B064-CCBC5B61BEFB}">
+    <text>MTOW em t</text>
+  </threadedComment>
+  <threadedComment ref="C59" dT="2021-06-07T18:32:51.41" personId="{172B4ACD-BB32-3A40-A6EE-78502C39DADA}" id="{6E62DECF-2988-4A4A-9803-744B9D3906AC}">
+    <text>Em cada container cabem 4 aviões, porém vários componentes serão integrados nos EUA, portanto considerei 70% do MTOW</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B232C13D-411F-C34C-8B06-A5C237365F81}">
   <dimension ref="A1:M129"/>
@@ -4577,9 +4742,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C712432D-C946-4E76-9C56-C65B4186EF49}">
   <dimension ref="A1:M118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -6746,8 +6911,8 @@
   <dimension ref="A1:M126"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -8903,9 +9068,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70E134E5-91A9-214F-A953-DB87B8BF84DC}">
   <dimension ref="A1:M115"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7:G9"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -11061,9 +11226,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D772B5C0-78A8-4453-9C12-C71D4E986150}">
   <dimension ref="A1:M139"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
+    <sheetView zoomScale="139" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -13532,4 +13697,2474 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C22AB5-D450-4C56-BC98-DADF57DC22A2}">
+  <dimension ref="A1:M139"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="7.109375" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="75.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="B1" s="67" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1">
+      <c r="A4" s="69" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" s="54">
+        <v>0.83</v>
+      </c>
+      <c r="D4" s="11">
+        <f>C4</f>
+        <v>0.83</v>
+      </c>
+      <c r="E4" s="11">
+        <f>C4</f>
+        <v>0.83</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1">
+      <c r="A5" s="69"/>
+      <c r="B5" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" s="54">
+        <v>1</v>
+      </c>
+      <c r="D5" s="11">
+        <f t="shared" ref="D5:D68" si="0">C5</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="11">
+        <f t="shared" ref="E5:E68" si="1">C5</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="69"/>
+      <c r="B6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="26">
+        <v>563.97</v>
+      </c>
+      <c r="D6" s="11">
+        <f t="shared" si="0"/>
+        <v>563.97</v>
+      </c>
+      <c r="E6" s="11">
+        <f t="shared" si="1"/>
+        <v>563.97</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="69"/>
+      <c r="B7" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="C7" s="54">
+        <v>1E-4</v>
+      </c>
+      <c r="D7" s="11">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+      <c r="E7" s="11">
+        <f t="shared" si="1"/>
+        <v>1E-4</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="69"/>
+      <c r="B8" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C8" s="54">
+        <v>1E-4</v>
+      </c>
+      <c r="D8" s="11">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+      <c r="E8" s="11">
+        <f t="shared" si="1"/>
+        <v>1E-4</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="I8">
+        <f>C7*C8*C9*C13</f>
+        <v>3.0666666666666664E-11</v>
+      </c>
+      <c r="J8">
+        <f>I8+I9</f>
+        <v>713978.75733333337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="69"/>
+      <c r="B9" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C9" s="54">
+        <v>1E-4</v>
+      </c>
+      <c r="D9" s="11">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+      <c r="E9" s="11">
+        <f t="shared" si="1"/>
+        <v>1E-4</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I9">
+        <f>C10*C11*C12*C13</f>
+        <v>713978.75733333337</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="69"/>
+      <c r="B10" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="C10" s="54">
+        <v>818</v>
+      </c>
+      <c r="D10" s="11">
+        <f t="shared" si="0"/>
+        <v>818</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" si="1"/>
+        <v>818</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="69"/>
+      <c r="B11" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C11" s="54">
+        <f>15.96/60</f>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="D11" s="11">
+        <f t="shared" si="0"/>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="E11" s="11">
+        <f t="shared" si="1"/>
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="69"/>
+      <c r="B12" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="C12" s="11">
+        <v>107</v>
+      </c>
+      <c r="D12" s="11">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+      <c r="E12" s="11">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="69"/>
+      <c r="B13" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="11">
+        <f>AVERAGE(23,38,31)</f>
+        <v>30.666666666666668</v>
+      </c>
+      <c r="D13" s="11">
+        <f t="shared" si="0"/>
+        <v>30.666666666666668</v>
+      </c>
+      <c r="E13" s="11">
+        <f t="shared" si="1"/>
+        <v>30.666666666666668</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="69"/>
+      <c r="B14" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="54">
+        <f>(8204*0.43)</f>
+        <v>3527.72</v>
+      </c>
+      <c r="D14" s="11">
+        <f t="shared" si="0"/>
+        <v>3527.72</v>
+      </c>
+      <c r="E14" s="11">
+        <f t="shared" si="1"/>
+        <v>3527.72</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="69"/>
+      <c r="B15" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="54">
+        <f>(8204*0.57)</f>
+        <v>4676.28</v>
+      </c>
+      <c r="D15" s="11">
+        <f t="shared" si="0"/>
+        <v>4676.28</v>
+      </c>
+      <c r="E15" s="11">
+        <f t="shared" si="1"/>
+        <v>4676.28</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="69"/>
+      <c r="B16" s="57" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="50">
+        <v>15</v>
+      </c>
+      <c r="D16" s="11">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E16" s="11">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="69"/>
+      <c r="B17" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="50">
+        <v>70</v>
+      </c>
+      <c r="D17" s="11">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="E17" s="11">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="69"/>
+      <c r="B18" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" s="50">
+        <v>15</v>
+      </c>
+      <c r="D18" s="11">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E18" s="11">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="69"/>
+      <c r="B19" s="57" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="50">
+        <v>10</v>
+      </c>
+      <c r="D19" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E19" s="11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="69"/>
+      <c r="B20" s="57" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="50">
+        <v>20</v>
+      </c>
+      <c r="D20" s="11">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E20" s="11">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="70"/>
+      <c r="B21" s="57" t="s">
+        <v>133</v>
+      </c>
+      <c r="C21" s="50">
+        <v>70</v>
+      </c>
+      <c r="D21" s="11">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="E21" s="11">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="30" customFormat="1" ht="14.7" customHeight="1">
+      <c r="A22" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="44">
+        <f>214.17*C26</f>
+        <v>510.43849999999998</v>
+      </c>
+      <c r="D22" s="44">
+        <f t="shared" si="0"/>
+        <v>510.43849999999998</v>
+      </c>
+      <c r="E22" s="44">
+        <f t="shared" si="1"/>
+        <v>510.43849999999998</v>
+      </c>
+      <c r="F22" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="30" customFormat="1">
+      <c r="A23" s="72"/>
+      <c r="B23" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="44">
+        <f>0.38*C26</f>
+        <v>0.90566666666666662</v>
+      </c>
+      <c r="D23" s="44">
+        <f t="shared" si="0"/>
+        <v>0.90566666666666662</v>
+      </c>
+      <c r="E23" s="44">
+        <f t="shared" si="1"/>
+        <v>0.90566666666666662</v>
+      </c>
+      <c r="F23" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" s="45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="30" customFormat="1">
+      <c r="A24" s="72"/>
+      <c r="B24" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="44">
+        <f>1.5*C26</f>
+        <v>3.5750000000000002</v>
+      </c>
+      <c r="D24" s="44">
+        <f t="shared" si="0"/>
+        <v>3.5750000000000002</v>
+      </c>
+      <c r="E24" s="44">
+        <f t="shared" si="1"/>
+        <v>3.5750000000000002</v>
+      </c>
+      <c r="F24" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="45" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="14.55" customHeight="1">
+      <c r="A25" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="46">
+        <f>5*12</f>
+        <v>60</v>
+      </c>
+      <c r="D25" s="46">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="E25" s="46">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="F25" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="74"/>
+      <c r="B26" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="24">
+        <f>(10+26+43+43+21)/C25</f>
+        <v>2.3833333333333333</v>
+      </c>
+      <c r="D26" s="24">
+        <f t="shared" si="0"/>
+        <v>2.3833333333333333</v>
+      </c>
+      <c r="E26" s="24">
+        <f t="shared" si="1"/>
+        <v>2.3833333333333333</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="74"/>
+      <c r="B27" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C27" s="54">
+        <f>750*3</f>
+        <v>2250</v>
+      </c>
+      <c r="D27" s="24">
+        <f t="shared" si="0"/>
+        <v>2250</v>
+      </c>
+      <c r="E27" s="24">
+        <f t="shared" si="1"/>
+        <v>2250</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="74"/>
+      <c r="B28" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="54">
+        <f>(750+170+310+60)*3</f>
+        <v>3870</v>
+      </c>
+      <c r="D28" s="24">
+        <f t="shared" si="0"/>
+        <v>3870</v>
+      </c>
+      <c r="E28" s="24">
+        <f t="shared" si="1"/>
+        <v>3870</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="74"/>
+      <c r="B29" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="C29" s="59">
+        <v>1</v>
+      </c>
+      <c r="D29" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E29" s="33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F29" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="G29" s="34" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="74"/>
+      <c r="B30" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="C30" s="59">
+        <v>8</v>
+      </c>
+      <c r="D30" s="33">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E30" s="33">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="F30" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="G30" s="34" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="74"/>
+      <c r="B31" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="24">
+        <v>3</v>
+      </c>
+      <c r="D31" s="24">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E31" s="24">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="74"/>
+      <c r="B32" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="24">
+        <v>1</v>
+      </c>
+      <c r="D32" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E32" s="24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="74"/>
+      <c r="B33" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="24">
+        <v>1000</v>
+      </c>
+      <c r="D33" s="24">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="E33" s="24">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="14.55" customHeight="1">
+      <c r="A34" s="75" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="54">
+        <f>0.29+0.09+0.16</f>
+        <v>0.54</v>
+      </c>
+      <c r="D34" s="12">
+        <f t="shared" si="0"/>
+        <v>0.54</v>
+      </c>
+      <c r="E34" s="12">
+        <f t="shared" si="1"/>
+        <v>0.54</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="14.55" customHeight="1">
+      <c r="A35" s="76"/>
+      <c r="B35" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="54">
+        <f>0.2</f>
+        <v>0.2</v>
+      </c>
+      <c r="D35" s="12">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="E35" s="12">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="76"/>
+      <c r="B36" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C36" s="54">
+        <f>0.26</f>
+        <v>0.26</v>
+      </c>
+      <c r="D36" s="12">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+      <c r="E36" s="12">
+        <f t="shared" si="1"/>
+        <v>0.26</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="76"/>
+      <c r="B37" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="54">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D37" s="12">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E37" s="12">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="76"/>
+      <c r="B38" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="54">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D38" s="12">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E38" s="12">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="76"/>
+      <c r="B39" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="54">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D39" s="12">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E39" s="12">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="76"/>
+      <c r="B40" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="12">
+        <v>1.25</v>
+      </c>
+      <c r="D40" s="12">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="E40" s="12">
+        <f t="shared" si="1"/>
+        <v>1.25</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="76"/>
+      <c r="B41" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="12">
+        <v>1.25</v>
+      </c>
+      <c r="D41" s="12">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="E41" s="12">
+        <f t="shared" si="1"/>
+        <v>1.25</v>
+      </c>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="76"/>
+      <c r="B42" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C42" s="12">
+        <v>1</v>
+      </c>
+      <c r="D42" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E42" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="76"/>
+      <c r="B43" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="12">
+        <v>1.2</v>
+      </c>
+      <c r="D43" s="12">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="E43" s="12">
+        <f t="shared" si="1"/>
+        <v>1.2</v>
+      </c>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="76"/>
+      <c r="B44" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="12">
+        <v>1</v>
+      </c>
+      <c r="D44" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E44" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="76"/>
+      <c r="B45" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="12">
+        <v>1</v>
+      </c>
+      <c r="D45" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E45" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="14.55" customHeight="1">
+      <c r="A46" s="77" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" s="38">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D46" s="38">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E46" s="38">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F46" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="G46" s="39" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="14.55" customHeight="1">
+      <c r="A47" s="78"/>
+      <c r="B47" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="C47" s="38">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D47" s="38">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E47" s="38">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F47" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="G47" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="I47" s="51"/>
+      <c r="J47" s="51"/>
+      <c r="K47" s="51"/>
+      <c r="L47" s="51"/>
+      <c r="M47" s="51"/>
+    </row>
+    <row r="48" spans="1:13" ht="14.55" customHeight="1">
+      <c r="A48" s="78"/>
+      <c r="B48" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" s="38">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D48" s="38">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E48" s="38">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F48" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="G48" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="I48" s="51"/>
+      <c r="J48" s="51"/>
+      <c r="K48" s="51"/>
+      <c r="L48" s="51"/>
+      <c r="M48" s="51"/>
+    </row>
+    <row r="49" spans="1:13" ht="14.55" customHeight="1">
+      <c r="A49" s="78"/>
+      <c r="B49" s="47" t="s">
+        <v>194</v>
+      </c>
+      <c r="C49" s="53">
+        <f>4.44*$C$22</f>
+        <v>2266.3469399999999</v>
+      </c>
+      <c r="D49" s="38">
+        <f t="shared" si="0"/>
+        <v>2266.3469399999999</v>
+      </c>
+      <c r="E49" s="38">
+        <f t="shared" si="1"/>
+        <v>2266.3469399999999</v>
+      </c>
+      <c r="F49" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="G49" s="39" t="s">
+        <v>195</v>
+      </c>
+      <c r="H49" s="48"/>
+      <c r="I49" s="51"/>
+      <c r="J49" s="52"/>
+      <c r="K49" s="52"/>
+      <c r="L49" s="52"/>
+      <c r="M49" s="51"/>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="78"/>
+      <c r="B50" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50" s="36">
+        <f>0.00444*C28</f>
+        <v>17.1828</v>
+      </c>
+      <c r="D50" s="36">
+        <f t="shared" si="0"/>
+        <v>17.1828</v>
+      </c>
+      <c r="E50" s="36">
+        <f t="shared" si="1"/>
+        <v>17.1828</v>
+      </c>
+      <c r="F50" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="G50" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="I50" s="51"/>
+      <c r="J50" s="51"/>
+      <c r="K50" s="51"/>
+      <c r="L50" s="51"/>
+      <c r="M50" s="51"/>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="78"/>
+      <c r="B51" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" s="36">
+        <f>0.00356*C28</f>
+        <v>13.777199999999999</v>
+      </c>
+      <c r="D51" s="36">
+        <f t="shared" si="0"/>
+        <v>13.777199999999999</v>
+      </c>
+      <c r="E51" s="36">
+        <f t="shared" si="1"/>
+        <v>13.777199999999999</v>
+      </c>
+      <c r="F51" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="G51" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="I51" s="51"/>
+      <c r="J51" s="51"/>
+      <c r="K51" s="51"/>
+      <c r="L51" s="51"/>
+      <c r="M51" s="51"/>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="78"/>
+      <c r="B52" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" s="36">
+        <f>0.000015*C28</f>
+        <v>5.8050000000000004E-2</v>
+      </c>
+      <c r="D52" s="36">
+        <f t="shared" si="0"/>
+        <v>5.8050000000000004E-2</v>
+      </c>
+      <c r="E52" s="36">
+        <f t="shared" si="1"/>
+        <v>5.8050000000000004E-2</v>
+      </c>
+      <c r="F52" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="G52" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="I52" s="51"/>
+      <c r="J52" s="51"/>
+      <c r="K52" s="51"/>
+      <c r="L52" s="51"/>
+      <c r="M52" s="51"/>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="79"/>
+      <c r="B53" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="C53" s="36">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D53" s="36">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E53" s="36">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F53" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="G53" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="I53" s="51"/>
+      <c r="J53" s="51"/>
+      <c r="K53" s="51"/>
+      <c r="L53" s="51"/>
+      <c r="M53" s="51"/>
+    </row>
+    <row r="54" spans="1:13" ht="14.55" customHeight="1">
+      <c r="A54" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="54">
+        <f>800</f>
+        <v>800</v>
+      </c>
+      <c r="D54" s="15">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="E54" s="15">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+      <c r="F54" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="61"/>
+      <c r="B55" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55" s="15">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D55" s="15">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E55" s="15">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F55" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" s="61"/>
+      <c r="B56" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56" s="15">
+        <f>AVERAGE(1808,8554,18177,14838,1304)</f>
+        <v>8936.2000000000007</v>
+      </c>
+      <c r="D56" s="15">
+        <f t="shared" si="0"/>
+        <v>8936.2000000000007</v>
+      </c>
+      <c r="E56" s="15">
+        <f t="shared" si="1"/>
+        <v>8936.2000000000007</v>
+      </c>
+      <c r="F56" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" s="61"/>
+      <c r="B57" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" s="54">
+        <f>1150/1000</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D57" s="15">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E57" s="15">
+        <f t="shared" si="1"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F57" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G57" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" s="61"/>
+      <c r="B58" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C58" s="15">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D58" s="15">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E58" s="15">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F58" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G58" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59" s="61"/>
+      <c r="B59" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C59" s="54">
+        <f>(C57*0.7)*4</f>
+        <v>3.2199999999999998</v>
+      </c>
+      <c r="D59" s="15">
+        <f t="shared" si="0"/>
+        <v>3.2199999999999998</v>
+      </c>
+      <c r="E59" s="15">
+        <f t="shared" si="1"/>
+        <v>3.2199999999999998</v>
+      </c>
+      <c r="F59" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G59" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="14.55" customHeight="1">
+      <c r="A60" s="62" t="s">
+        <v>215</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="C60" s="55">
+        <f>36.52/7937</f>
+        <v>4.6012347234471469E-3</v>
+      </c>
+      <c r="D60" s="25">
+        <f t="shared" si="0"/>
+        <v>4.6012347234471469E-3</v>
+      </c>
+      <c r="E60" s="25">
+        <f t="shared" si="1"/>
+        <v>4.6012347234471469E-3</v>
+      </c>
+      <c r="F60" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G60" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="K60" s="13"/>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" s="63"/>
+      <c r="B61" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C61" s="55">
+        <f>83.48/7937</f>
+        <v>1.0517827894670531E-2</v>
+      </c>
+      <c r="D61" s="18">
+        <f t="shared" si="0"/>
+        <v>1.0517827894670531E-2</v>
+      </c>
+      <c r="E61" s="18">
+        <f t="shared" si="1"/>
+        <v>1.0517827894670531E-2</v>
+      </c>
+      <c r="F61" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G61" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="K61" s="13"/>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="A62" s="63"/>
+      <c r="B62" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="C62" s="55">
+        <f>41.74/7937</f>
+        <v>5.2589139473352654E-3</v>
+      </c>
+      <c r="D62" s="18">
+        <f t="shared" si="0"/>
+        <v>5.2589139473352654E-3</v>
+      </c>
+      <c r="E62" s="18">
+        <f t="shared" si="1"/>
+        <v>5.2589139473352654E-3</v>
+      </c>
+      <c r="F62" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G62" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="K62" s="13"/>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63" s="63"/>
+      <c r="B63" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="C63" s="55">
+        <f>36.52/7937</f>
+        <v>4.6012347234471469E-3</v>
+      </c>
+      <c r="D63" s="18">
+        <f t="shared" si="0"/>
+        <v>4.6012347234471469E-3</v>
+      </c>
+      <c r="E63" s="18">
+        <f t="shared" si="1"/>
+        <v>4.6012347234471469E-3</v>
+      </c>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="K63" s="13"/>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" s="63"/>
+      <c r="B64" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="C64" s="55">
+        <f>52.17/7937</f>
+        <v>6.5730124732266606E-3</v>
+      </c>
+      <c r="D64" s="18">
+        <f t="shared" si="0"/>
+        <v>6.5730124732266606E-3</v>
+      </c>
+      <c r="E64" s="18">
+        <f t="shared" si="1"/>
+        <v>6.5730124732266606E-3</v>
+      </c>
+      <c r="F64" s="19"/>
+      <c r="G64" s="19"/>
+      <c r="K64" s="13"/>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" s="63"/>
+      <c r="B65" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C65" s="55">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D65" s="18">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E65" s="18">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F65" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="G65" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="K65" s="13"/>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" s="63"/>
+      <c r="B66" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="C66" s="55">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D66" s="18">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E66" s="18">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F66" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="G66" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="K66" s="13"/>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" s="63"/>
+      <c r="B67" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="C67" s="55">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D67" s="18">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E67" s="18">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F67" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="G67" s="19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" s="63"/>
+      <c r="B68" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="C68" s="55">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D68" s="18">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E68" s="18">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F68" s="21"/>
+      <c r="G68" s="19"/>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" s="63"/>
+      <c r="B69" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="C69" s="55">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D69" s="18">
+        <f t="shared" ref="D69:D104" si="2">C69</f>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E69" s="18">
+        <f t="shared" ref="E69:E132" si="3">C69</f>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F69" s="21"/>
+      <c r="G69" s="19"/>
+    </row>
+    <row r="70" spans="1:11" ht="14.55" customHeight="1">
+      <c r="A70" s="62" t="s">
+        <v>216</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C70" s="55">
+        <f>46.96/7937</f>
+        <v>5.9165931712233839E-3</v>
+      </c>
+      <c r="D70" s="25">
+        <f t="shared" si="2"/>
+        <v>5.9165931712233839E-3</v>
+      </c>
+      <c r="E70" s="25">
+        <f t="shared" si="3"/>
+        <v>5.9165931712233839E-3</v>
+      </c>
+      <c r="F70" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G70" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="K70" s="13"/>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" s="63"/>
+      <c r="B71" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="C71" s="55">
+        <f>86.6/7937</f>
+        <v>1.0910923522741589E-2</v>
+      </c>
+      <c r="D71" s="18">
+        <f t="shared" si="2"/>
+        <v>1.0910923522741589E-2</v>
+      </c>
+      <c r="E71" s="18">
+        <f t="shared" si="3"/>
+        <v>1.0910923522741589E-2</v>
+      </c>
+      <c r="F71" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G71" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="K71" s="13"/>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" s="63"/>
+      <c r="B72" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="C72" s="55">
+        <f>36.52/7937</f>
+        <v>4.6012347234471469E-3</v>
+      </c>
+      <c r="D72" s="18">
+        <f t="shared" si="2"/>
+        <v>4.6012347234471469E-3</v>
+      </c>
+      <c r="E72" s="18">
+        <f t="shared" si="3"/>
+        <v>4.6012347234471469E-3</v>
+      </c>
+      <c r="F72" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G72" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="K72" s="13"/>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" s="63"/>
+      <c r="B73" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="C73" s="55">
+        <f>46.96/7937</f>
+        <v>5.9165931712233839E-3</v>
+      </c>
+      <c r="D73" s="18">
+        <f t="shared" si="2"/>
+        <v>5.9165931712233839E-3</v>
+      </c>
+      <c r="E73" s="18">
+        <f t="shared" si="3"/>
+        <v>5.9165931712233839E-3</v>
+      </c>
+      <c r="F73" s="19"/>
+      <c r="G73" s="19"/>
+      <c r="K73" s="13"/>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74" s="63"/>
+      <c r="B74" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="C74" s="55">
+        <f>55/7937</f>
+        <v>6.9295703666372686E-3</v>
+      </c>
+      <c r="D74" s="18">
+        <f t="shared" si="2"/>
+        <v>6.9295703666372686E-3</v>
+      </c>
+      <c r="E74" s="18">
+        <f t="shared" si="3"/>
+        <v>6.9295703666372686E-3</v>
+      </c>
+      <c r="F74" s="19"/>
+      <c r="G74" s="19"/>
+      <c r="K74" s="13"/>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75" s="63"/>
+      <c r="B75" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="C75" s="55">
+        <f>5.61*60</f>
+        <v>336.6</v>
+      </c>
+      <c r="D75" s="18">
+        <f t="shared" si="2"/>
+        <v>336.6</v>
+      </c>
+      <c r="E75" s="18">
+        <f t="shared" si="3"/>
+        <v>336.6</v>
+      </c>
+      <c r="F75" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="G75" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="K75" s="13"/>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" s="63"/>
+      <c r="B76" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="C76" s="55">
+        <f>0.55*60</f>
+        <v>33</v>
+      </c>
+      <c r="D76" s="18">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="E76" s="18">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="F76" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="G76" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="K76" s="13"/>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77" s="63"/>
+      <c r="B77" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="C77" s="56">
+        <f>2.5*60</f>
+        <v>150</v>
+      </c>
+      <c r="D77" s="18">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="E77" s="18">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="F77" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="G77" s="19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" s="63"/>
+      <c r="B78" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="C78" s="56">
+        <f>11.6*60</f>
+        <v>696</v>
+      </c>
+      <c r="D78" s="18">
+        <f t="shared" si="2"/>
+        <v>696</v>
+      </c>
+      <c r="E78" s="18">
+        <f t="shared" si="3"/>
+        <v>696</v>
+      </c>
+      <c r="F78" s="21"/>
+      <c r="G78" s="19"/>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79" s="63"/>
+      <c r="B79" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="C79" s="56">
+        <f>3.72*60</f>
+        <v>223.20000000000002</v>
+      </c>
+      <c r="D79" s="18">
+        <f t="shared" si="2"/>
+        <v>223.20000000000002</v>
+      </c>
+      <c r="E79" s="18">
+        <f t="shared" si="3"/>
+        <v>223.20000000000002</v>
+      </c>
+      <c r="F79" s="21"/>
+      <c r="G79" s="19"/>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80" s="63"/>
+      <c r="B80" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C80" s="27">
+        <v>2</v>
+      </c>
+      <c r="D80" s="18">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E80" s="18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F80" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="G80" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="K80" s="13"/>
+    </row>
+    <row r="81" spans="1:11" ht="14.55" customHeight="1">
+      <c r="A81" s="63"/>
+      <c r="B81" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="C81" s="27">
+        <v>0.95</v>
+      </c>
+      <c r="D81" s="18">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="E81" s="18">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="F81" s="21"/>
+      <c r="G81" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="K81" s="13"/>
+    </row>
+    <row r="82" spans="1:11" ht="14.55" customHeight="1">
+      <c r="A82" s="63"/>
+      <c r="B82" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="C82" s="27">
+        <v>10</v>
+      </c>
+      <c r="D82" s="18">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="E82" s="18">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="F82" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="G82" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="K82" s="13"/>
+    </row>
+    <row r="83" spans="1:11" ht="14.55" customHeight="1">
+      <c r="A83" s="63"/>
+      <c r="B83" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C83" s="18">
+        <v>2.3315789473684214</v>
+      </c>
+      <c r="D83" s="18">
+        <f t="shared" si="2"/>
+        <v>2.3315789473684214</v>
+      </c>
+      <c r="E83" s="18">
+        <f t="shared" si="3"/>
+        <v>2.3315789473684214</v>
+      </c>
+      <c r="F83" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G83" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="K83" s="13"/>
+    </row>
+    <row r="84" spans="1:11">
+      <c r="A84" s="63"/>
+      <c r="B84" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C84" s="18">
+        <v>4.4784688995215309E-2</v>
+      </c>
+      <c r="D84" s="18">
+        <f t="shared" si="2"/>
+        <v>4.4784688995215309E-2</v>
+      </c>
+      <c r="E84" s="18">
+        <f t="shared" si="3"/>
+        <v>4.4784688995215309E-2</v>
+      </c>
+      <c r="F84" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G84" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="K84" s="13"/>
+    </row>
+    <row r="85" spans="1:11">
+      <c r="A85" s="63"/>
+      <c r="B85" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C85" s="18">
+        <v>4.2497607655502394</v>
+      </c>
+      <c r="D85" s="18">
+        <f t="shared" si="2"/>
+        <v>4.2497607655502394</v>
+      </c>
+      <c r="E85" s="18">
+        <f t="shared" si="3"/>
+        <v>4.2497607655502394</v>
+      </c>
+      <c r="F85" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G85" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="K85" s="13"/>
+    </row>
+    <row r="86" spans="1:11">
+      <c r="A86" s="64"/>
+      <c r="B86" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C86" s="18">
+        <v>6</v>
+      </c>
+      <c r="D86" s="18">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E86" s="18">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="F86" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G86" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="K86" s="13"/>
+    </row>
+    <row r="87" spans="1:11" ht="14.55" customHeight="1">
+      <c r="A87" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="B87" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C87" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="D87" s="41">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="E87" s="41">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="F87" s="42"/>
+      <c r="G87" s="42" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
+      <c r="A88" s="66"/>
+      <c r="B88" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C88" s="49">
+        <v>0.2</v>
+      </c>
+      <c r="D88" s="41">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="E88" s="41">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="F88" s="42"/>
+      <c r="G88" s="42" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
+      <c r="A89" s="66"/>
+      <c r="B89" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C89" s="49">
+        <v>0.2</v>
+      </c>
+      <c r="D89" s="41">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="E89" s="41">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="F89" s="42"/>
+      <c r="G89" s="42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
+      <c r="A90" s="66"/>
+      <c r="B90" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C90" s="50">
+        <v>0.2</v>
+      </c>
+      <c r="D90" s="41">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="E90" s="41">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="F90" s="42"/>
+      <c r="G90" s="42" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
+      <c r="A91" s="66"/>
+      <c r="B91" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C91" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="D91" s="41">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="E91" s="41">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="F91" s="42"/>
+      <c r="G91" s="42" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
+      <c r="A92" s="66"/>
+      <c r="B92" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="C92" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="D92" s="41">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="E92" s="41">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="F92" s="42"/>
+      <c r="G92" s="42" t="s">
+        <v>191</v>
+      </c>
+      <c r="K92" s="13"/>
+    </row>
+    <row r="93" spans="1:11">
+      <c r="A93" s="66"/>
+      <c r="B93" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C93" s="50">
+        <v>0.25</v>
+      </c>
+      <c r="D93" s="41">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="E93" s="41">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="F93" s="42"/>
+      <c r="G93" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="K93" s="13"/>
+    </row>
+    <row r="94" spans="1:11">
+      <c r="A94" s="66"/>
+      <c r="B94" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C94" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="D94" s="41">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="E94" s="41">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="F94" s="42"/>
+      <c r="G94" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="K94" s="13"/>
+    </row>
+    <row r="95" spans="1:11">
+      <c r="A95" s="66"/>
+      <c r="B95" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C95" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="D95" s="41">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="E95" s="41">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="F95" s="42"/>
+      <c r="G95" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="K95" s="13"/>
+    </row>
+    <row r="96" spans="1:11">
+      <c r="A96" s="66"/>
+      <c r="B96" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C96" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="D96" s="41">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="E96" s="41">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="F96" s="42"/>
+      <c r="G96" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="K96" s="13"/>
+    </row>
+    <row r="97" spans="1:11">
+      <c r="A97" s="66"/>
+      <c r="B97" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C97" s="50">
+        <v>0.45</v>
+      </c>
+      <c r="D97" s="41">
+        <f t="shared" si="2"/>
+        <v>0.45</v>
+      </c>
+      <c r="E97" s="41">
+        <f t="shared" si="3"/>
+        <v>0.45</v>
+      </c>
+      <c r="F97" s="42"/>
+      <c r="G97" s="42" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
+      <c r="A98" s="66"/>
+      <c r="B98" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="C98" s="50">
+        <v>0.45</v>
+      </c>
+      <c r="D98" s="41">
+        <f t="shared" si="2"/>
+        <v>0.45</v>
+      </c>
+      <c r="E98" s="41">
+        <f t="shared" si="3"/>
+        <v>0.45</v>
+      </c>
+      <c r="F98" s="42"/>
+      <c r="G98" s="42" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
+      <c r="A99" s="66"/>
+      <c r="B99" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C99" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="D99" s="41">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="E99" s="41">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="F99" s="42"/>
+      <c r="G99" s="42" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
+      <c r="A100" s="66"/>
+      <c r="B100" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C100" s="49">
+        <v>0.7</v>
+      </c>
+      <c r="D100" s="41">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+      <c r="E100" s="41">
+        <f t="shared" si="3"/>
+        <v>0.7</v>
+      </c>
+      <c r="F100" s="42"/>
+      <c r="G100" s="42" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
+      <c r="A101" s="66"/>
+      <c r="B101" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C101" s="49">
+        <v>0.7</v>
+      </c>
+      <c r="D101" s="41">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+      <c r="E101" s="41">
+        <f t="shared" si="3"/>
+        <v>0.7</v>
+      </c>
+      <c r="F101" s="42"/>
+      <c r="G101" s="42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
+      <c r="A102" s="66"/>
+      <c r="B102" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C102" s="49">
+        <v>0.7</v>
+      </c>
+      <c r="D102" s="41">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+      <c r="E102" s="41">
+        <f t="shared" si="3"/>
+        <v>0.7</v>
+      </c>
+      <c r="F102" s="42"/>
+      <c r="G102" s="42" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
+      <c r="A103" s="66"/>
+      <c r="B103" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C103" s="49">
+        <v>0.05</v>
+      </c>
+      <c r="D103" s="41">
+        <f t="shared" si="2"/>
+        <v>0.05</v>
+      </c>
+      <c r="E103" s="41">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+      <c r="F103" s="42"/>
+      <c r="G103" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="K103" s="13"/>
+    </row>
+    <row r="104" spans="1:11">
+      <c r="A104" s="66"/>
+      <c r="B104" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="C104" s="49">
+        <v>0.05</v>
+      </c>
+      <c r="D104" s="41">
+        <f t="shared" si="2"/>
+        <v>0.05</v>
+      </c>
+      <c r="E104" s="41">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+      <c r="F104" s="42"/>
+      <c r="G104" s="42" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="121" spans="11:11">
+      <c r="K121" s="13"/>
+    </row>
+    <row r="125" spans="11:11">
+      <c r="K125" s="13"/>
+    </row>
+    <row r="126" spans="11:11">
+      <c r="K126" s="13"/>
+    </row>
+    <row r="127" spans="11:11">
+      <c r="K127" s="13"/>
+    </row>
+    <row r="128" spans="11:11">
+      <c r="K128" s="13"/>
+    </row>
+    <row r="129" spans="11:11">
+      <c r="K129" s="13"/>
+    </row>
+    <row r="130" spans="11:11">
+      <c r="K130" s="13"/>
+    </row>
+    <row r="131" spans="11:11">
+      <c r="K131" s="13"/>
+    </row>
+    <row r="132" spans="11:11">
+      <c r="K132" s="13"/>
+    </row>
+    <row r="133" spans="11:11">
+      <c r="K133" s="13"/>
+    </row>
+    <row r="134" spans="11:11">
+      <c r="K134" s="13"/>
+    </row>
+    <row r="135" spans="11:11">
+      <c r="K135" s="13"/>
+    </row>
+    <row r="136" spans="11:11">
+      <c r="K136" s="13"/>
+    </row>
+    <row r="137" spans="11:11">
+      <c r="K137" s="13"/>
+    </row>
+    <row r="139" spans="11:11">
+      <c r="K139" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A54:A59"/>
+    <mergeCell ref="A60:A69"/>
+    <mergeCell ref="A70:A86"/>
+    <mergeCell ref="A87:A104"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="A4:A21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A33"/>
+    <mergeCell ref="A34:A45"/>
+    <mergeCell ref="A46:A53"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>